<commit_message>
tinggal buat velocity @zoy
</commit_message>
<xml_diff>
--- a/KRISLAM Perpustakaan.xlsx
+++ b/KRISLAM Perpustakaan.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Sm4\Pengembangan Perangkat Lunak Tangkas (Ibu Mustika Ulina)\project-perpustakaan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50446A03-A213-4E22-88D5-365D22A3735D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE50E10B-D340-41EC-8927-A4E3DD505F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{6267A1EC-14CF-41E6-99C5-673D034BD963}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{6267A1EC-14CF-41E6-99C5-673D034BD963}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint Backlog" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -138,6 +139,48 @@
   </si>
   <si>
     <t>saya mendapatkan informasi terbaru mengenai keanggotaan</t>
+  </si>
+  <si>
+    <t>SPRINT BACKLOG</t>
+  </si>
+  <si>
+    <t>Tasks</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Membuat datar anggota</t>
+  </si>
+  <si>
+    <t>Membuat daftar kategori buku</t>
+  </si>
+  <si>
+    <t>Memastikan buku bersih dan tersusun rapi</t>
+  </si>
+  <si>
+    <t>Membuat kotak saran</t>
+  </si>
+  <si>
+    <t>Memiliki kartu Keanggotaan</t>
+  </si>
+  <si>
+    <t>Membuat kata kunci pencarian buku</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -176,18 +219,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFA500"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -210,23 +253,87 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,18 +657,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F46BB30-3C90-418A-82F8-E64DBF455B16}">
   <dimension ref="B5:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="6.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="45.28515625" customWidth="1"/>
+    <col min="4" max="4" width="48.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69.7109375" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -575,354 +682,354 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="4">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
+      <c r="B8" s="1">
         <v>2</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="4">
+      <c r="B9" s="1">
         <v>3</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="4">
+      <c r="B10" s="1">
         <v>4</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>14</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>15</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>16</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>17</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
         <v>18</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
         <v>19</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="4">
-        <v>5</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="4">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
         <v>20</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="4" t="s">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="4">
-        <v>7</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
         <v>22</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
         <v>23</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="4">
-        <v>8</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="4">
-        <v>9</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="4">
-        <v>10</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="4">
-        <v>11</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="4">
-        <v>12</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="4">
-        <v>13</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="4">
-        <v>14</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="4">
-        <v>15</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="4">
-        <v>16</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="4">
-        <v>17</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="4">
-        <v>18</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="4">
-        <v>19</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="4">
-        <v>20</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="4">
-        <v>21</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="4">
-        <v>22</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="4">
-        <v>23</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -931,4 +1038,180 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E8FE28-9745-479A-8240-23C4D7DBC060}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.140625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8">
+        <v>4</v>
+      </c>
+      <c r="D6" s="8">
+        <v>3</v>
+      </c>
+      <c r="E6" s="8">
+        <v>2</v>
+      </c>
+      <c r="F6" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="8">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
velocity udah, tinggal finishing
</commit_message>
<xml_diff>
--- a/KRISLAM Perpustakaan.xlsx
+++ b/KRISLAM Perpustakaan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Sm4\Pengembangan Perangkat Lunak Tangkas (Ibu Mustika Ulina)\project-perpustakaan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE50E10B-D340-41EC-8927-A4E3DD505F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3184D8-DBC2-4AA2-B446-86B4CFD91C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{6267A1EC-14CF-41E6-99C5-673D034BD963}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -204,7 +207,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,6 +229,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,34 +303,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -334,6 +325,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -356,6 +374,1045 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ID"/>
+              <a:t>Velocity</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint Backlog'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Monday</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint Backlog'!$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-96B8-42AD-A1F9-4B6DECA88691}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint Backlog'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tuesday</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint Backlog'!$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-96B8-42AD-A1F9-4B6DECA88691}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint Backlog'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Wednesday</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint Backlog'!$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-96B8-42AD-A1F9-4B6DECA88691}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint Backlog'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Thursday</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint Backlog'!$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-96B8-42AD-A1F9-4B6DECA88691}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint Backlog'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Friday</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint Backlog'!$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-96B8-42AD-A1F9-4B6DECA88691}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1007335839"/>
+        <c:axId val="1007338335"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1007335839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1007338335"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1007338335"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1007335839"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8390B3D2-4437-4FF8-A504-865F46F4C38E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -655,9 +1712,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F46BB30-3C90-418A-82F8-E64DBF455B16}">
-  <dimension ref="B5:G29"/>
+  <dimension ref="B5:G16"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -672,32 +1729,32 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -900,136 +1957,6 @@
       <c r="G16" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
-        <v>11</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
-        <v>12</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1">
-        <v>13</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="1">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="1">
-        <v>15</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1">
-        <v>16</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="1">
-        <v>17</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="1">
-        <v>18</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="1">
-        <v>19</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="1">
-        <v>20</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="1">
-        <v>21</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="1">
-        <v>22</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="1">
-        <v>23</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1042,15 +1969,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E8FE28-9745-479A-8240-23C4D7DBC060}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.140625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" style="5" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -1059,153 +1986,178 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="7"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="14">
         <v>1</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="3">
         <v>1</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="3">
         <v>1</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="3">
         <v>4</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="3">
         <v>3</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="3">
         <v>2</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="3">
         <v>1</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="3">
         <v>1</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="3">
         <v>1</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="3">
         <v>1</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="3">
         <v>1</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="3">
         <v>1</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="3">
         <v>1</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="16">
+        <f>SUM(B3:B8)</f>
+        <v>5</v>
+      </c>
+      <c r="C9" s="16">
+        <f t="shared" ref="C9:F9" si="0">SUM(C3:C8)</f>
+        <v>7</v>
+      </c>
+      <c r="D9" s="16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E9" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F9" s="16">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1213,5 +2165,7 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>